<commit_message>
Commit 2019-04-22 kl. 12:41
</commit_message>
<xml_diff>
--- a/Administration/Utgifter.xlsx
+++ b/Administration/Utgifter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Administration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_cjonasl\Leander\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56FE00F-6DD1-4BCB-A4FD-22EDAFB6448B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D800CA5A-BD41-47DE-AEC6-F010DB48930B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{093D95A9-BDCB-4607-BCAA-8EA444957F99}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
   <si>
     <t>Bananer</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Mobiltelefon</t>
+  </si>
+  <si>
+    <t>Skurduk</t>
+  </si>
+  <si>
+    <t>Toalettborste</t>
+  </si>
+  <si>
+    <t>Raklödder</t>
+  </si>
+  <si>
+    <t>Kaffe</t>
   </si>
 </sst>
 </file>
@@ -636,11 +648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCF06E2-471F-4482-AF28-8713356AEBBD}">
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AI39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +666,7 @@
       </c>
       <c r="B1" s="7">
         <f>SUM(F3:AI3)</f>
-        <v>289.39999999999998</v>
+        <v>348.08</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -664,7 +676,7 @@
       </c>
       <c r="B2" s="7">
         <f>B1/B3</f>
-        <v>17.023529411764706</v>
+        <v>18.32</v>
       </c>
       <c r="C2" s="5"/>
       <c r="F2" s="2" t="s">
@@ -763,7 +775,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" s="3" t="s">
@@ -839,11 +851,11 @@
       </c>
       <c r="W3" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34.33</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24.349999999999998</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" si="0"/>
@@ -896,7 +908,7 @@
       </c>
       <c r="E4" s="4">
         <f>SUM(F4:AI4)</f>
-        <v>5.57</v>
+        <v>5.9700000000000006</v>
       </c>
       <c r="F4" s="4">
         <v>0.5</v>
@@ -918,6 +930,9 @@
       </c>
       <c r="T4" s="4">
         <v>1</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -926,7 +941,7 @@
       </c>
       <c r="E5" s="4">
         <f>SUM(F5:AI5)</f>
-        <v>5.9899999999999993</v>
+        <v>6.9799999999999995</v>
       </c>
       <c r="F5">
         <v>0.95</v>
@@ -953,6 +968,12 @@
       <c r="V5">
         <v>0.55000000000000004</v>
       </c>
+      <c r="W5">
+        <v>0.49</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -981,7 +1002,7 @@
       </c>
       <c r="E7" s="4">
         <f>SUM(F7:AI7)</f>
-        <v>33.9</v>
+        <v>39.65</v>
       </c>
       <c r="H7" s="4">
         <v>3</v>
@@ -994,6 +1015,10 @@
       </c>
       <c r="S7">
         <v>11.65</v>
+      </c>
+      <c r="X7">
+        <f>2+2+1.75</f>
+        <v>5.75</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -1001,8 +1026,8 @@
         <v>35</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" ref="E8:E35" si="1">SUM(F8:AI8)</f>
-        <v>5.09</v>
+        <f t="shared" ref="E8:E39" si="1">SUM(F8:AI8)</f>
+        <v>6.9799999999999995</v>
       </c>
       <c r="I8">
         <v>1.85</v>
@@ -1011,6 +1036,9 @@
         <v>1.35</v>
       </c>
       <c r="R8">
+        <v>1.89</v>
+      </c>
+      <c r="W8">
         <v>1.89</v>
       </c>
     </row>
@@ -1038,7 +1066,7 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>49.8</v>
+        <v>71.949999999999989</v>
       </c>
       <c r="J10" s="4">
         <v>5.9</v>
@@ -1051,6 +1079,9 @@
       </c>
       <c r="T10" s="4">
         <v>4.2</v>
+      </c>
+      <c r="W10">
+        <v>22.15</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -1059,10 +1090,13 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
       <c r="J11" s="4">
         <v>0.8</v>
+      </c>
+      <c r="W11" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -1071,7 +1105,7 @@
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>5.73</v>
+        <v>6.83</v>
       </c>
       <c r="J12">
         <v>0.89</v>
@@ -1089,6 +1123,9 @@
         <v>0.99</v>
       </c>
       <c r="V12" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X12" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1110,7 +1147,7 @@
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>2.5999999999999996</v>
+        <v>3.6499999999999995</v>
       </c>
       <c r="K14">
         <f>0.7+0.85</f>
@@ -1119,6 +1156,9 @@
       <c r="R14">
         <v>1.05</v>
       </c>
+      <c r="W14">
+        <v>1.05</v>
+      </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
@@ -1126,13 +1166,16 @@
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>4.99</v>
+        <v>6.99</v>
       </c>
       <c r="K15" s="4">
         <v>2</v>
       </c>
       <c r="R15">
         <v>2.99</v>
+      </c>
+      <c r="X15" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -1141,31 +1184,37 @@
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K16" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>3.35</v>
       </c>
       <c r="K17" s="4">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="X17" s="4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.65</v>
       </c>
       <c r="K18" s="4">
         <v>0.1</v>
@@ -1173,14 +1222,17 @@
       <c r="P18" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="X18">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>4.28</v>
+        <v>6.28</v>
       </c>
       <c r="M19" s="4">
         <v>1</v>
@@ -1194,8 +1246,11 @@
       <c r="T19">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>49</v>
       </c>
@@ -1207,7 +1262,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>50</v>
       </c>
@@ -1222,7 +1277,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>51</v>
       </c>
@@ -1237,7 +1292,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>52</v>
       </c>
@@ -1252,7 +1307,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>53</v>
       </c>
@@ -1264,19 +1319,23 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>54</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>5.4</v>
       </c>
       <c r="P25" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="X25" s="4">
+        <f>1.75+1.45</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>55</v>
       </c>
@@ -1288,7 +1347,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>56</v>
       </c>
@@ -1303,7 +1362,7 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D28" s="9" t="s">
         <v>57</v>
       </c>
@@ -1315,7 +1374,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>58</v>
       </c>
@@ -1327,19 +1386,22 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>4.3499999999999996</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="R30">
         <v>4.3499999999999996</v>
       </c>
-    </row>
-    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W30">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
         <v>60</v>
       </c>
@@ -1351,7 +1413,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>63</v>
       </c>
@@ -1375,7 +1437,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>64</v>
       </c>
@@ -1387,7 +1449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>65</v>
       </c>
@@ -1397,6 +1459,54 @@
       </c>
       <c r="T35" s="4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="X39" s="4">
+        <v>6.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit 2019-04-22 kl. 22:48
</commit_message>
<xml_diff>
--- a/Administration/Utgifter.xlsx
+++ b/Administration/Utgifter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_cjonasl\Leander\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D800CA5A-BD41-47DE-AEC6-F010DB48930B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3000FD6-B089-40E0-8802-BECCD425E896}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{093D95A9-BDCB-4607-BCAA-8EA444957F99}"/>
   </bookViews>
@@ -651,8 +651,8 @@
   <dimension ref="A1:AI39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <pane xSplit="5" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +679,7 @@
         <v>18.32</v>
       </c>
       <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>